<commit_message>
Modificacion de los scripts
</commit_message>
<xml_diff>
--- a/Diccionario de datos/dic_Titulos.xlsx
+++ b/Diccionario de datos/dic_Titulos.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,58 +434,56 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>¡Nop!</t>
-        </is>
+      <c r="A1" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tierra Santa</t>
+          <t>Dragon Ball Super: Super Heroe</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>After: Amor infinito</t>
+          <t>Tren Bala</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Desastre en el vuelo Us57</t>
+          <t>Minions Nace un Villano</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dragon Ball Super: Super Héroe</t>
+          <t>Escalera al Infierno</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tren bala</t>
+          <t>DC Liga de Super Mascotas</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DC Liga de Supermascotas</t>
+          <t>Thor Amor y Trueno</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>El teléfono negro</t>
+          <t>Seventeen World Tour BE THE SUN- Houston LIVE VIEWING</t>
         </is>
       </c>
     </row>
@@ -487,63 +497,98 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Thor: Amor y trueno</t>
+          <t>El Telefono Negro</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Minions: Nace un villano</t>
+          <t>Alarido</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cadejo blanco</t>
+          <t>Bestia</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Escalera al infierno</t>
+          <t>Top Gun Maverick</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Berta soy yo</t>
+          <t>Cambio de Planes</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ámbar</t>
+          <t>Jurassic World Dominio</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bestia</t>
+          <t>2022 Festivales y Muestras</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Alarido</t>
+          <t>Berta Soy Yo</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Indómita salvaje</t>
+          <t>Indómita Salvaje</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Exodo La Ultima Marea</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Persiguiendo un Sueño</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>El Sacrificio</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Buena Suerte Leo Grande</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>El Fotógrafo De Minamata</t>
         </is>
       </c>
     </row>

</xml_diff>